<commit_message>
write sum of donations made to the nominator per committee-member to a new worksheet
</commit_message>
<xml_diff>
--- a/donor_committee_member_matches.xlsx
+++ b/donor_committee_member_matches.xlsx
@@ -9,13 +9,14 @@
   <sheets>
     <sheet name="last_name_match" sheetId="1" r:id="rId1"/>
     <sheet name="full_name_match" sheetId="2" r:id="rId2"/>
+    <sheet name="sum_donations_to_nominator" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6751" uniqueCount="1092">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6936" uniqueCount="1092">
   <si>
     <t>Committee Member</t>
   </si>
@@ -24400,6 +24401,9 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
         <v>4</v>
       </c>
     </row>
@@ -28582,6 +28586,1031 @@
         <v>18</v>
       </c>
       <c r="E247" t="s">
+        <v>41</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C92"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2">
+        <v>100</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3">
+        <v>1000</v>
+      </c>
+      <c r="C3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B4">
+        <v>1000</v>
+      </c>
+      <c r="C4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B5">
+        <v>100</v>
+      </c>
+      <c r="C5" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" t="s">
+        <v>79</v>
+      </c>
+      <c r="B6">
+        <v>1000</v>
+      </c>
+      <c r="C6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" t="s">
+        <v>92</v>
+      </c>
+      <c r="B7">
+        <v>200</v>
+      </c>
+      <c r="C7" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" t="s">
+        <v>150</v>
+      </c>
+      <c r="B8">
+        <v>1000</v>
+      </c>
+      <c r="C8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" t="s">
+        <v>152</v>
+      </c>
+      <c r="B9">
+        <v>100</v>
+      </c>
+      <c r="C9" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" t="s">
+        <v>156</v>
+      </c>
+      <c r="B10">
+        <v>1250</v>
+      </c>
+      <c r="C10" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" t="s">
+        <v>160</v>
+      </c>
+      <c r="B11">
+        <v>2000</v>
+      </c>
+      <c r="C11" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" t="s">
+        <v>178</v>
+      </c>
+      <c r="B12">
+        <v>100</v>
+      </c>
+      <c r="C12" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" t="s">
+        <v>195</v>
+      </c>
+      <c r="B13">
+        <v>100</v>
+      </c>
+      <c r="C13" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" t="s">
+        <v>230</v>
+      </c>
+      <c r="B14">
+        <v>250</v>
+      </c>
+      <c r="C14" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" t="s">
+        <v>242</v>
+      </c>
+      <c r="B15">
+        <v>103.48</v>
+      </c>
+      <c r="C15" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" t="s">
+        <v>259</v>
+      </c>
+      <c r="B16">
+        <v>500</v>
+      </c>
+      <c r="C16" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" t="s">
+        <v>302</v>
+      </c>
+      <c r="B17">
+        <v>200</v>
+      </c>
+      <c r="C17" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" t="s">
+        <v>328</v>
+      </c>
+      <c r="B18">
+        <v>200</v>
+      </c>
+      <c r="C18" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" t="s">
+        <v>331</v>
+      </c>
+      <c r="B19">
+        <v>50</v>
+      </c>
+      <c r="C19" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" t="s">
+        <v>352</v>
+      </c>
+      <c r="B20">
+        <v>250</v>
+      </c>
+      <c r="C20" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" t="s">
+        <v>376</v>
+      </c>
+      <c r="B21">
+        <v>150</v>
+      </c>
+      <c r="C21" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" t="s">
+        <v>386</v>
+      </c>
+      <c r="B22">
+        <v>1000</v>
+      </c>
+      <c r="C22" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" t="s">
+        <v>390</v>
+      </c>
+      <c r="B23">
+        <v>1250</v>
+      </c>
+      <c r="C23" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" t="s">
+        <v>395</v>
+      </c>
+      <c r="B24">
+        <v>50</v>
+      </c>
+      <c r="C24" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25" t="s">
+        <v>406</v>
+      </c>
+      <c r="B25">
+        <v>201.99</v>
+      </c>
+      <c r="C25" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26" t="s">
+        <v>412</v>
+      </c>
+      <c r="B26">
+        <v>100</v>
+      </c>
+      <c r="C26" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27" t="s">
+        <v>421</v>
+      </c>
+      <c r="B27">
+        <v>100</v>
+      </c>
+      <c r="C27" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28" t="s">
+        <v>434</v>
+      </c>
+      <c r="B28">
+        <v>100</v>
+      </c>
+      <c r="C28" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="A29" t="s">
+        <v>456</v>
+      </c>
+      <c r="B29">
+        <v>500</v>
+      </c>
+      <c r="C29" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
+      <c r="A30" t="s">
+        <v>460</v>
+      </c>
+      <c r="B30">
+        <v>500</v>
+      </c>
+      <c r="C30" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="A31" t="s">
+        <v>474</v>
+      </c>
+      <c r="B31">
+        <v>100</v>
+      </c>
+      <c r="C31" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
+      <c r="A32" t="s">
+        <v>478</v>
+      </c>
+      <c r="B32">
+        <v>200</v>
+      </c>
+      <c r="C32" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
+      <c r="A33" t="s">
+        <v>505</v>
+      </c>
+      <c r="B33">
+        <v>1500</v>
+      </c>
+      <c r="C33" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
+      <c r="A34" t="s">
+        <v>532</v>
+      </c>
+      <c r="B34">
+        <v>200</v>
+      </c>
+      <c r="C34" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3">
+      <c r="A35" t="s">
+        <v>534</v>
+      </c>
+      <c r="B35">
+        <v>2500</v>
+      </c>
+      <c r="C35" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
+      <c r="A36" t="s">
+        <v>556</v>
+      </c>
+      <c r="B36">
+        <v>100</v>
+      </c>
+      <c r="C36" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3">
+      <c r="A37" t="s">
+        <v>572</v>
+      </c>
+      <c r="B37">
+        <v>1000</v>
+      </c>
+      <c r="C37" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3">
+      <c r="A38" t="s">
+        <v>574</v>
+      </c>
+      <c r="B38">
+        <v>5000</v>
+      </c>
+      <c r="C38" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3">
+      <c r="A39" t="s">
+        <v>578</v>
+      </c>
+      <c r="B39">
+        <v>5000</v>
+      </c>
+      <c r="C39" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3">
+      <c r="A40" t="s">
+        <v>607</v>
+      </c>
+      <c r="B40">
+        <v>50</v>
+      </c>
+      <c r="C40" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3">
+      <c r="A41" t="s">
+        <v>611</v>
+      </c>
+      <c r="B41">
+        <v>750</v>
+      </c>
+      <c r="C41" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3">
+      <c r="A42" t="s">
+        <v>628</v>
+      </c>
+      <c r="B42">
+        <v>350</v>
+      </c>
+      <c r="C42" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3">
+      <c r="A43" t="s">
+        <v>633</v>
+      </c>
+      <c r="B43">
+        <v>257.94</v>
+      </c>
+      <c r="C43" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3">
+      <c r="A44" t="s">
+        <v>667</v>
+      </c>
+      <c r="B44">
+        <v>200</v>
+      </c>
+      <c r="C44" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3">
+      <c r="A45" t="s">
+        <v>669</v>
+      </c>
+      <c r="B45">
+        <v>100</v>
+      </c>
+      <c r="C45" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3">
+      <c r="A46" t="s">
+        <v>675</v>
+      </c>
+      <c r="B46">
+        <v>1000</v>
+      </c>
+      <c r="C46" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3">
+      <c r="A47" t="s">
+        <v>683</v>
+      </c>
+      <c r="B47">
+        <v>500</v>
+      </c>
+      <c r="C47" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3">
+      <c r="A48" t="s">
+        <v>702</v>
+      </c>
+      <c r="B48">
+        <v>450</v>
+      </c>
+      <c r="C48" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3">
+      <c r="A49" t="s">
+        <v>726</v>
+      </c>
+      <c r="B49">
+        <v>250</v>
+      </c>
+      <c r="C49" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3">
+      <c r="A50" t="s">
+        <v>731</v>
+      </c>
+      <c r="B50">
+        <v>1000</v>
+      </c>
+      <c r="C50" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3">
+      <c r="A51" t="s">
+        <v>738</v>
+      </c>
+      <c r="B51">
+        <v>350</v>
+      </c>
+      <c r="C51" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3">
+      <c r="A52" t="s">
+        <v>742</v>
+      </c>
+      <c r="B52">
+        <v>500</v>
+      </c>
+      <c r="C52" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3">
+      <c r="A53" t="s">
+        <v>748</v>
+      </c>
+      <c r="B53">
+        <v>500</v>
+      </c>
+      <c r="C53" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3">
+      <c r="A54" t="s">
+        <v>759</v>
+      </c>
+      <c r="B54">
+        <v>100</v>
+      </c>
+      <c r="C54" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3">
+      <c r="A55" t="s">
+        <v>766</v>
+      </c>
+      <c r="B55">
+        <v>50</v>
+      </c>
+      <c r="C55" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3">
+      <c r="A56" t="s">
+        <v>778</v>
+      </c>
+      <c r="B56">
+        <v>75</v>
+      </c>
+      <c r="C56" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3">
+      <c r="A57" t="s">
+        <v>782</v>
+      </c>
+      <c r="B57">
+        <v>50</v>
+      </c>
+      <c r="C57" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3">
+      <c r="A58" t="s">
+        <v>791</v>
+      </c>
+      <c r="B58">
+        <v>500</v>
+      </c>
+      <c r="C58" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3">
+      <c r="A59" t="s">
+        <v>793</v>
+      </c>
+      <c r="B59">
+        <v>155.47</v>
+      </c>
+      <c r="C59" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3">
+      <c r="A60" t="s">
+        <v>795</v>
+      </c>
+      <c r="B60">
+        <v>100</v>
+      </c>
+      <c r="C60" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3">
+      <c r="A61" t="s">
+        <v>809</v>
+      </c>
+      <c r="B61">
+        <v>100</v>
+      </c>
+      <c r="C61" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3">
+      <c r="A62" t="s">
+        <v>683</v>
+      </c>
+      <c r="B62">
+        <v>500</v>
+      </c>
+      <c r="C62" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3">
+      <c r="A63" t="s">
+        <v>815</v>
+      </c>
+      <c r="B63">
+        <v>500</v>
+      </c>
+      <c r="C63" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3">
+      <c r="A64" t="s">
+        <v>840</v>
+      </c>
+      <c r="B64">
+        <v>1000</v>
+      </c>
+      <c r="C64" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3">
+      <c r="A65" t="s">
+        <v>844</v>
+      </c>
+      <c r="B65">
+        <v>15000</v>
+      </c>
+      <c r="C65" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3">
+      <c r="A66" t="s">
+        <v>857</v>
+      </c>
+      <c r="B66">
+        <v>50</v>
+      </c>
+      <c r="C66" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3">
+      <c r="A67" t="s">
+        <v>859</v>
+      </c>
+      <c r="B67">
+        <v>500</v>
+      </c>
+      <c r="C67" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3">
+      <c r="A68" t="s">
+        <v>862</v>
+      </c>
+      <c r="B68">
+        <v>350</v>
+      </c>
+      <c r="C68" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3">
+      <c r="A69" t="s">
+        <v>878</v>
+      </c>
+      <c r="B69">
+        <v>1000</v>
+      </c>
+      <c r="C69" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3">
+      <c r="A70" t="s">
+        <v>910</v>
+      </c>
+      <c r="B70">
+        <v>1000</v>
+      </c>
+      <c r="C70" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3">
+      <c r="A71" t="s">
+        <v>913</v>
+      </c>
+      <c r="B71">
+        <v>500</v>
+      </c>
+      <c r="C71" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3">
+      <c r="A72" t="s">
+        <v>917</v>
+      </c>
+      <c r="B72">
+        <v>600</v>
+      </c>
+      <c r="C72" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3">
+      <c r="A73" t="s">
+        <v>918</v>
+      </c>
+      <c r="B73">
+        <v>250</v>
+      </c>
+      <c r="C73" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3">
+      <c r="A74" t="s">
+        <v>878</v>
+      </c>
+      <c r="B74">
+        <v>1000</v>
+      </c>
+      <c r="C74" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3">
+      <c r="A75" t="s">
+        <v>926</v>
+      </c>
+      <c r="B75">
+        <v>500</v>
+      </c>
+      <c r="C75" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3">
+      <c r="A76" t="s">
+        <v>927</v>
+      </c>
+      <c r="B76">
+        <v>50</v>
+      </c>
+      <c r="C76" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3">
+      <c r="A77" t="s">
+        <v>972</v>
+      </c>
+      <c r="B77">
+        <v>47.2</v>
+      </c>
+      <c r="C77" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3">
+      <c r="A78" t="s">
+        <v>983</v>
+      </c>
+      <c r="B78">
+        <v>332.2</v>
+      </c>
+      <c r="C78" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3">
+      <c r="A79" t="s">
+        <v>986</v>
+      </c>
+      <c r="B79">
+        <v>250</v>
+      </c>
+      <c r="C79" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3">
+      <c r="A80" t="s">
+        <v>994</v>
+      </c>
+      <c r="B80">
+        <v>100</v>
+      </c>
+      <c r="C80" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3">
+      <c r="A81" t="s">
+        <v>996</v>
+      </c>
+      <c r="B81">
+        <v>625</v>
+      </c>
+      <c r="C81" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3">
+      <c r="A82" t="s">
+        <v>998</v>
+      </c>
+      <c r="B82">
+        <v>100</v>
+      </c>
+      <c r="C82" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3">
+      <c r="A83" t="s">
+        <v>1003</v>
+      </c>
+      <c r="B83">
+        <v>500</v>
+      </c>
+      <c r="C83" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3">
+      <c r="A84" t="s">
+        <v>1006</v>
+      </c>
+      <c r="B84">
+        <v>1000</v>
+      </c>
+      <c r="C84" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3">
+      <c r="A85" t="s">
+        <v>1009</v>
+      </c>
+      <c r="B85">
+        <v>500</v>
+      </c>
+      <c r="C85" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3">
+      <c r="A86" t="s">
+        <v>1028</v>
+      </c>
+      <c r="B86">
+        <v>51.99</v>
+      </c>
+      <c r="C86" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3">
+      <c r="A87" t="s">
+        <v>1046</v>
+      </c>
+      <c r="B87">
+        <v>51.99</v>
+      </c>
+      <c r="C87" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3">
+      <c r="A88" t="s">
+        <v>1048</v>
+      </c>
+      <c r="B88">
+        <v>350</v>
+      </c>
+      <c r="C88" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3">
+      <c r="A89" t="s">
+        <v>1055</v>
+      </c>
+      <c r="B89">
+        <v>350</v>
+      </c>
+      <c r="C89" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3">
+      <c r="A90" t="s">
+        <v>1056</v>
+      </c>
+      <c r="B90">
+        <v>100</v>
+      </c>
+      <c r="C90" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3">
+      <c r="A91" t="s">
+        <v>1066</v>
+      </c>
+      <c r="B91">
+        <v>250</v>
+      </c>
+      <c r="C91" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3">
+      <c r="A92" t="s">
+        <v>1069</v>
+      </c>
+      <c r="B92">
+        <v>100</v>
+      </c>
+      <c r="C92" t="s">
         <v>41</v>
       </c>
     </row>

</xml_diff>